<commit_message>
Add officiels, competitions and clubs
</commit_message>
<xml_diff>
--- a/Officiels.xlsx
+++ b/Officiels.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="226">
   <si>
     <t>Club</t>
   </si>
@@ -34,15 +34,21 @@
     <t>A.S DRAGUIGNAN NATATION</t>
   </si>
   <si>
+    <t>AC HYÈRES</t>
+  </si>
+  <si>
+    <t>AC CANNES</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
     <t>AMSL FRÉJUS</t>
   </si>
   <si>
     <t>AQUATIC CLUB DE MENTON</t>
   </si>
   <si>
-    <t>06</t>
-  </si>
-  <si>
     <t>AS CACHALOTS SIX-FOURS</t>
   </si>
   <si>
@@ -97,6 +103,9 @@
     <t>US ST-TROPEZ</t>
   </si>
   <si>
+    <t>CLUB OMNISPORTS DE VALBONNE</t>
+  </si>
+  <si>
     <t>Nom</t>
   </si>
   <si>
@@ -115,12 +124,27 @@
     <t>AIRAUD Sophie</t>
   </si>
   <si>
+    <t>BARALE Sylvain</t>
+  </si>
+  <si>
+    <t>BARRALIS Patrick</t>
+  </si>
+  <si>
     <t>BARROT Gilbert</t>
   </si>
   <si>
+    <t>BAUSSY Charles</t>
+  </si>
+  <si>
     <t>BEAUMONT Frédéric</t>
   </si>
   <si>
+    <t>BELIN Philippe</t>
+  </si>
+  <si>
+    <t>BENARD Deborah</t>
+  </si>
+  <si>
     <t>BERTAUX Yann</t>
   </si>
   <si>
@@ -136,12 +160,21 @@
     <t>BONY Christine</t>
   </si>
   <si>
+    <t>BORGOGNO Eric</t>
+  </si>
+  <si>
     <t>BOTTERO Annie</t>
   </si>
   <si>
     <t>BRIAND David</t>
   </si>
   <si>
+    <t>BRIMAULT Joël</t>
+  </si>
+  <si>
+    <t>CACI Jean-Philippe</t>
+  </si>
+  <si>
     <t>CALATAYUD Lionel</t>
   </si>
   <si>
@@ -157,6 +190,9 @@
     <t>CARLES Corinne</t>
   </si>
   <si>
+    <t>CHAPUIS Annick</t>
+  </si>
+  <si>
     <t>CHERRIERE Martine</t>
   </si>
   <si>
@@ -166,72 +202,189 @@
     <t>CLAMENS Sophie</t>
   </si>
   <si>
+    <t>COLPAERT Christelle</t>
+  </si>
+  <si>
+    <t>COSTANTINI Isabelle</t>
+  </si>
+  <si>
     <t>COURTIN Richard</t>
   </si>
   <si>
     <t>COUTANT Isabelle</t>
   </si>
   <si>
+    <t>DAGUET Magali</t>
+  </si>
+  <si>
     <t>DAL MASO Christine</t>
   </si>
   <si>
+    <t>DALLE Frederique</t>
+  </si>
+  <si>
+    <t>DANJOU Lola</t>
+  </si>
+  <si>
+    <t>DEAGE Isabelle</t>
+  </si>
+  <si>
+    <t>DECOMBIS Marlene</t>
+  </si>
+  <si>
+    <t>DECOMBIS Olivier</t>
+  </si>
+  <si>
+    <t>DEGAUGUE Franck</t>
+  </si>
+  <si>
     <t>DELACROIX Romane</t>
   </si>
   <si>
     <t>DIONISI Sébastien</t>
   </si>
   <si>
+    <t>DORI Damien</t>
+  </si>
+  <si>
+    <t>DUBOST Jerome</t>
+  </si>
+  <si>
     <t>DUGARDIN Hugues</t>
   </si>
   <si>
+    <t>EYMENIER Nicolas</t>
+  </si>
+  <si>
     <t>FELIX Ariane</t>
   </si>
   <si>
     <t>FLECHE Eric</t>
   </si>
   <si>
+    <t>FLORENT Jerome</t>
+  </si>
+  <si>
+    <t>FREAUD PARRET Mireille</t>
+  </si>
+  <si>
     <t>GALLO GEROLD Karyn</t>
   </si>
   <si>
     <t>GARRO Francoise</t>
   </si>
   <si>
+    <t>GAUBERT Pierre</t>
+  </si>
+  <si>
+    <t>GELFMANN Erwan</t>
+  </si>
+  <si>
+    <t>GELFMANN Gwenaelle</t>
+  </si>
+  <si>
+    <t>GELFMANN Laurent</t>
+  </si>
+  <si>
+    <t>GELFMANN Soizic</t>
+  </si>
+  <si>
     <t>GIBSON Herbert</t>
   </si>
   <si>
+    <t>GIOANNI Jean-Marc</t>
+  </si>
+  <si>
     <t>GIORDANENGO Jean-Louis</t>
   </si>
   <si>
     <t>GIOVANETTI Nadege</t>
   </si>
   <si>
+    <t>GIOVANNETTI Lucas</t>
+  </si>
+  <si>
+    <t>GUIRADO Jerome</t>
+  </si>
+  <si>
     <t>HEMERY Emmanuelle</t>
   </si>
   <si>
+    <t>HESSE Christelle</t>
+  </si>
+  <si>
     <t>JIGUET David</t>
   </si>
   <si>
     <t>JIGUET Sandrine</t>
   </si>
   <si>
+    <t>JULIAN J-François</t>
+  </si>
+  <si>
+    <t>KHALIL Souad</t>
+  </si>
+  <si>
+    <t>KITCHING Anna</t>
+  </si>
+  <si>
+    <t>LAFOSSE Gregory</t>
+  </si>
+  <si>
+    <t>LAGIER Alain</t>
+  </si>
+  <si>
+    <t>LAGIER Dominique</t>
+  </si>
+  <si>
     <t>LAHANA Didier</t>
   </si>
   <si>
+    <t>LAKCHAL Alain</t>
+  </si>
+  <si>
+    <t>LAMBREGHTS Jean-Philippe</t>
+  </si>
+  <si>
     <t>LE LAY Nathalie</t>
   </si>
   <si>
     <t>LEBON Christophe</t>
   </si>
   <si>
+    <t>LECOMTE Annie</t>
+  </si>
+  <si>
+    <t>LEMASSON Pascal</t>
+  </si>
+  <si>
+    <t>LENICA Francis</t>
+  </si>
+  <si>
     <t>LEONARDI Ingrid</t>
   </si>
   <si>
     <t>LHERMITTE Morgan</t>
   </si>
   <si>
+    <t>LIOGIER Marc</t>
+  </si>
+  <si>
+    <t>LIOGIER Marie-Ange</t>
+  </si>
+  <si>
     <t>LOISY Stéphanie</t>
   </si>
   <si>
+    <t>MAITRE Nathalie</t>
+  </si>
+  <si>
+    <t>MANSIER Herve</t>
+  </si>
+  <si>
+    <t>MARINO Eric</t>
+  </si>
+  <si>
     <t>MARTIN Patrice</t>
   </si>
   <si>
@@ -241,6 +394,9 @@
     <t>MEYER Stephanie</t>
   </si>
   <si>
+    <t>MIGUET Patrice</t>
+  </si>
+  <si>
     <t>MILLE Nathalie</t>
   </si>
   <si>
@@ -262,6 +418,12 @@
     <t>NECTOUX Ivan</t>
   </si>
   <si>
+    <t>OLLIVIER Karen</t>
+  </si>
+  <si>
+    <t>PARIS HERITIER Claire</t>
+  </si>
+  <si>
     <t>PEREZ Stephane</t>
   </si>
   <si>
@@ -271,12 +433,18 @@
     <t>PERRIER Christine</t>
   </si>
   <si>
+    <t>PHILIPPOT Stéphane</t>
+  </si>
+  <si>
     <t>PIERRE Nathalie</t>
   </si>
   <si>
     <t>PRAILLET Gerard</t>
   </si>
   <si>
+    <t>PRAT Laurent</t>
+  </si>
+  <si>
     <t>REBERT Albert</t>
   </si>
   <si>
@@ -292,12 +460,42 @@
     <t>ROBERT Alain</t>
   </si>
   <si>
+    <t>ROGER Sophie</t>
+  </si>
+  <si>
     <t>ROSSO Jean-Jacques</t>
   </si>
   <si>
+    <t>ROUSSEAU Béatrice</t>
+  </si>
+  <si>
+    <t>SAINTON Sara</t>
+  </si>
+  <si>
+    <t>SASSELLI Cédric</t>
+  </si>
+  <si>
+    <t>SASSELLI Lola</t>
+  </si>
+  <si>
+    <t>SCHLATTER Sandra</t>
+  </si>
+  <si>
     <t>SELLET Peggy</t>
   </si>
   <si>
+    <t>SEZIONALE Gilles</t>
+  </si>
+  <si>
+    <t>SOREL Alan</t>
+  </si>
+  <si>
+    <t>VAMBRE Angelique</t>
+  </si>
+  <si>
+    <t>VANMOEN Isabelle</t>
+  </si>
+  <si>
     <t>VAROQUIER Stephane</t>
   </si>
   <si>
@@ -307,6 +505,9 @@
     <t>VIORA PUYO Valerie</t>
   </si>
   <si>
+    <t>WARLOP Veronique</t>
+  </si>
+  <si>
     <t>XALLE Christelle</t>
   </si>
   <si>
@@ -319,60 +520,63 @@
     <t>Niveau</t>
   </si>
   <si>
+    <t>Délégué fédéral</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Juge-Arbitre</t>
+  </si>
+  <si>
+    <t>Juges de nage</t>
+  </si>
+  <si>
+    <t>Starter</t>
+  </si>
+  <si>
     <t>Chambre d'appel</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
+    <t>Contrôleur de virages</t>
+  </si>
+  <si>
+    <t>Contrôleur de virages en chef</t>
+  </si>
+  <si>
+    <t>Juge d'arrivée</t>
+  </si>
+  <si>
     <t>Chronométreur</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>Contrôleur de virages</t>
-  </si>
-  <si>
-    <t>Contrôleur de virages en chef</t>
+    <t>Coordonnateur</t>
+  </si>
+  <si>
+    <t>Gestion extraNat</t>
   </si>
   <si>
     <t>Inscrit sans fonction</t>
   </si>
   <si>
-    <t>Juge d'arrivée</t>
-  </si>
-  <si>
-    <t>Juge-Arbitre</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Juges de nage</t>
+    <t>Ramasseur de Fiches</t>
+  </si>
+  <si>
+    <t>Secrétariat</t>
+  </si>
+  <si>
+    <t>Speaker</t>
   </si>
   <si>
     <t>Jury d'appel</t>
   </si>
   <si>
-    <t>Ramasseur de Fiches</t>
-  </si>
-  <si>
-    <t>Secrétariat</t>
-  </si>
-  <si>
-    <t>Starter</t>
-  </si>
-  <si>
-    <t>Coordonnateur</t>
-  </si>
-  <si>
-    <t>Gestion extraNat</t>
-  </si>
-  <si>
-    <t>Speaker</t>
-  </si>
-  <si>
     <t>Numéro</t>
   </si>
   <si>
@@ -400,7 +604,13 @@
     <t>x</t>
   </si>
   <si>
+    <t>Interclubs poule A (Equipes)</t>
+  </si>
+  <si>
     <t>Interclubs poule B (Equipes)</t>
+  </si>
+  <si>
+    <t>Interclubs poule C (Equipes)</t>
   </si>
   <si>
     <t>Championnats départementaux 06 et 83 25m</t>
@@ -583,47 +793,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="17" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="17" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="17" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="17" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -704,16 +915,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="1" sqref="D10 F27"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -768,16 +979,16 @@
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
+      <c r="B7" s="3" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3" t="n">
-        <v>83</v>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -792,8 +1003,8 @@
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
+      <c r="B10" s="3" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -808,8 +1019,8 @@
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="3" t="n">
-        <v>83</v>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -824,8 +1035,8 @@
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
+      <c r="B14" s="3" t="n">
+        <v>83</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -864,8 +1075,8 @@
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="3" t="n">
-        <v>83</v>
+      <c r="B19" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -888,8 +1099,32 @@
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="3" t="n">
         <v>83</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -908,238 +1143,242 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D134"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>19</v>
-      </c>
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="4" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="4" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>42005</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>7</v>
-      </c>
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>42005</v>
-      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>42005</v>
-      </c>
-      <c r="D14" s="4" t="n">
-        <v>42005</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="4" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="4" t="n">
-        <v>42005</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="2"/>
+        <v>21</v>
+      </c>
       <c r="D17" s="4" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="4" t="n">
-        <v>42005</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>42005</v>
@@ -1150,20 +1389,22 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>42005</v>
@@ -1174,523 +1415,1251 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="C24" s="3"/>
       <c r="D24" s="4" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>14</v>
+      <c r="A25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4" t="n">
+        <v>42005</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C26" s="3"/>
       <c r="D26" s="4" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>4</v>
+      <c r="A29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D29" s="4" t="n">
+        <v>42005</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="D31" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="4" t="n">
-        <v>42005</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C33" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="C33" s="4" t="n">
+        <v>42005</v>
+      </c>
       <c r="D33" s="4" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>14</v>
+      <c r="A34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4" t="n">
+        <v>42005</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="C35" s="3"/>
       <c r="D35" s="4" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="C36" s="3"/>
       <c r="D36" s="4" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="4" t="n">
-        <v>42005</v>
-      </c>
-      <c r="D38" s="4" t="n">
-        <v>42005</v>
-      </c>
+      <c r="A38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="2"/>
+        <v>11</v>
+      </c>
       <c r="D39" s="4" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>14</v>
-      </c>
+      <c r="A43" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B48" s="0" t="s">
+      <c r="A48" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="4" t="n">
-        <v>42005</v>
-      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" s="4" t="n">
-        <v>42005</v>
-      </c>
-      <c r="D49" s="4" t="n">
-        <v>42005</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="C51" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D51" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="D52" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="4" t="n">
-        <v>42005</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="4" t="n">
-        <v>42005</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="4" t="n">
+        <v>42005</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C58" s="4" t="n">
-        <v>42005</v>
-      </c>
       <c r="D58" s="4" t="n">
         <v>42005</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C59" s="4" t="n">
-        <v>42005</v>
-      </c>
-      <c r="D59" s="4" t="n">
-        <v>42005</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D61" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="3"/>
+      <c r="D65" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="3"/>
+      <c r="D67" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="4" t="n">
-        <v>42005</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B61" s="2" t="s">
+      <c r="C68" s="3"/>
+      <c r="D68" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="4" t="n">
-        <v>42005</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B62" s="2" t="s">
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D72" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D73" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D76" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D77" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" s="3"/>
+      <c r="D79" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B63" s="0" t="s">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D86" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C87" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D87" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="4" t="n">
-        <v>42005</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B64" s="2" t="s">
+      <c r="C91" s="3"/>
+      <c r="D91" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" s="3"/>
+      <c r="D94" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D95" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C97" s="3"/>
+      <c r="D97" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C65" s="2"/>
-      <c r="D65" s="4" t="n">
-        <v>42005</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B66" s="2" t="s">
+      <c r="C98" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D98" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C102" s="3"/>
+      <c r="D102" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D104" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A105" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A106" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C66" s="2"/>
-      <c r="D66" s="4" t="n">
-        <v>42005</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B67" s="2" t="s">
+      <c r="C106" s="3"/>
+      <c r="D106" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A107" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A109" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A110" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C67" s="4" t="n">
-        <v>42005</v>
-      </c>
-      <c r="D67" s="4" t="n">
-        <v>42005</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B68" s="0" t="s">
+      <c r="C110" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D110" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A111" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D111" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A112" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C112" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D112" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A113" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113" s="3"/>
+      <c r="D113" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A114" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C114" s="3"/>
+      <c r="D114" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A115" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A116" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C116" s="3"/>
+      <c r="D116" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A117" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B69" s="2" t="s">
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A118" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C118" s="3"/>
+      <c r="D118" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A119" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D119" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A120" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" s="3"/>
+      <c r="D120" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A121" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A124" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C124" s="3"/>
+      <c r="D124" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A125" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C125" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D125" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A126" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A127" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C127" s="3"/>
+      <c r="D127" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A128" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A129" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C129" s="3"/>
+      <c r="D129" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="4" t="n">
-        <v>42005</v>
-      </c>
-      <c r="D69" s="4" t="n">
-        <v>42005</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="C130" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D130" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C132" s="3"/>
+      <c r="D132" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C133" s="4" t="n">
+        <v>42005</v>
+      </c>
+      <c r="D133" s="4" t="n">
+        <v>42005</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1708,143 +2677,151 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="D10 B10"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>99</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>100</v>
+        <v>167</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>101</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>102</v>
+        <v>168</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>103</v>
+        <v>169</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>101</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>106</v>
+        <v>173</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>107</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>108</v>
+        <v>174</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>107</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>175</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>111</v>
+        <v>178</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>99</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>113</v>
+        <v>180</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>114</v>
+        <v>181</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>101</v>
-      </c>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1862,35 +2839,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="1" sqref="D10 E10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>185</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>186</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>187</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>120</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1901,7 +2879,7 @@
         <v>42288</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>121</v>
+        <v>189</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -1914,7 +2892,7 @@
         <v>42288</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>121</v>
+        <v>189</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -1927,7 +2905,7 @@
         <v>42288</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>122</v>
+        <v>190</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1940,7 +2918,7 @@
         <v>42288</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>122</v>
+        <v>190</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -1953,397 +2931,431 @@
         <v>42295</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>123</v>
+        <v>191</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>124</v>
+        <v>192</v>
       </c>
       <c r="E6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
-        <v>34323</v>
+        <v>34321</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>42315</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>125</v>
+        <v>193</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>124</v>
+        <v>192</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
-        <v>33007</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>42330</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+        <v>34323</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>42315</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="n">
-        <v>42337</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>127</v>
+      <c r="A9" s="3" t="n">
+        <v>34325</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>42315</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" s="3"/>
+        <v>192</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
-        <v>35303</v>
-      </c>
-      <c r="B10" s="7" t="n">
-        <v>42344</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>124</v>
-      </c>
+        <v>33007</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>42330</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
-        <v>35207</v>
-      </c>
-      <c r="B11" s="4" t="n">
-        <v>42351</v>
+      <c r="A11" s="3"/>
+      <c r="B11" s="9" t="n">
+        <v>42337</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>197</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
-        <v>35205</v>
-      </c>
-      <c r="B12" s="4" t="n">
-        <v>42357</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>35303</v>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>42344</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
-        <v>33009</v>
-      </c>
-      <c r="B13" s="4" t="n">
-        <v>42358</v>
+        <v>35207</v>
+      </c>
+      <c r="B13" s="9" t="n">
+        <v>42351</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>131</v>
+        <v>199</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4" t="n">
-        <v>42386</v>
+      <c r="A14" s="3" t="n">
+        <v>35205</v>
+      </c>
+      <c r="B14" s="9" t="n">
+        <v>42357</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>132</v>
+        <v>200</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4" t="n">
-        <v>42386</v>
+      <c r="A15" s="3" t="n">
+        <v>33009</v>
+      </c>
+      <c r="B15" s="9" t="n">
+        <v>42358</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>133</v>
+        <v>201</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
-        <v>35711</v>
-      </c>
-      <c r="B16" s="4" t="n">
-        <v>42393</v>
+      <c r="A16" s="3"/>
+      <c r="B16" s="9" t="n">
+        <v>42386</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
-      <c r="B17" s="4" t="n">
-        <v>42400</v>
+      <c r="B17" s="9" t="n">
+        <v>42386</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>129</v>
+        <v>203</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4" t="n">
-        <v>42400</v>
+      <c r="A18" s="3" t="n">
+        <v>35711</v>
+      </c>
+      <c r="B18" s="9" t="n">
+        <v>42393</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>135</v>
+        <v>204</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
-      <c r="B19" s="4" t="n">
-        <v>42407</v>
+      <c r="B19" s="9" t="n">
+        <v>42400</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>136</v>
+        <v>199</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
-      <c r="B20" s="4" t="n">
-        <v>42427</v>
+      <c r="B20" s="9" t="n">
+        <v>42400</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>137</v>
+        <v>205</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
-      <c r="B21" s="4" t="n">
-        <v>42428</v>
+      <c r="B21" s="9" t="n">
+        <v>42407</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>138</v>
+        <v>206</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
-      <c r="B22" s="4" t="n">
-        <v>42435</v>
+      <c r="B22" s="9" t="n">
+        <v>42427</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>139</v>
+        <v>207</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3"/>
-      <c r="B23" s="4" t="n">
-        <v>42442</v>
+      <c r="B23" s="9" t="n">
+        <v>42428</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>140</v>
+        <v>208</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
-      <c r="B24" s="4" t="n">
-        <v>42449</v>
+      <c r="B24" s="9" t="n">
+        <v>42435</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>141</v>
+        <v>209</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
-      <c r="B25" s="4" t="n">
-        <v>42456</v>
+      <c r="B25" s="9" t="n">
+        <v>42442</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>142</v>
+        <v>210</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
-      <c r="B26" s="4" t="n">
-        <v>42462</v>
+      <c r="B26" s="9" t="n">
+        <v>42449</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>130</v>
+        <v>211</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
-      <c r="B27" s="4" t="n">
-        <v>42463</v>
+      <c r="B27" s="9" t="n">
+        <v>42456</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>143</v>
+        <v>212</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
-      <c r="B28" s="4" t="n">
-        <v>42470</v>
+      <c r="B28" s="9" t="n">
+        <v>42462</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
-      <c r="B29" s="4" t="n">
-        <v>42484</v>
+      <c r="B29" s="9" t="n">
+        <v>42463</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>145</v>
+        <v>213</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
-      <c r="B30" s="4" t="n">
-        <v>42498</v>
+      <c r="B30" s="9" t="n">
+        <v>42470</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>146</v>
+        <v>214</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
-      <c r="B31" s="4" t="n">
-        <v>42505</v>
+      <c r="B31" s="9" t="n">
+        <v>42484</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>147</v>
+        <v>215</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
-      <c r="B32" s="4" t="n">
-        <v>42512</v>
+      <c r="B32" s="9" t="n">
+        <v>42498</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>148</v>
+        <v>216</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
-      <c r="B33" s="4" t="n">
-        <v>42512</v>
+      <c r="B33" s="9" t="n">
+        <v>42505</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>149</v>
+        <v>217</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
-      <c r="B34" s="4" t="n">
-        <v>42526</v>
+      <c r="B34" s="9" t="n">
+        <v>42512</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>150</v>
+        <v>218</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
-      <c r="B35" s="4" t="n">
-        <v>42160</v>
+      <c r="B35" s="9" t="n">
+        <v>42512</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>151</v>
+        <v>219</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
-      <c r="B36" s="4" t="n">
-        <v>42167</v>
+      <c r="B36" s="9" t="n">
+        <v>42526</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>152</v>
+        <v>220</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
-      <c r="B37" s="4" t="n">
-        <v>42174</v>
+      <c r="B37" s="9" t="n">
+        <v>42160</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>153</v>
+        <v>221</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3"/>
-      <c r="B38" s="4" t="n">
-        <v>42174</v>
+      <c r="B38" s="9" t="n">
+        <v>42167</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>154</v>
+        <v>222</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
-      <c r="B39" s="4" t="n">
-        <v>42180</v>
+      <c r="B39" s="9" t="n">
+        <v>42174</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>155</v>
+        <v>223</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3"/>
+      <c r="B40" s="9" t="n">
+        <v>42174</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3"/>
+      <c r="B41" s="9" t="n">
+        <v>42180</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fix points calculation problem
</commit_message>
<xml_diff>
--- a/Officiels.xlsx
+++ b/Officiels.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Clubs" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="340">
   <si>
     <t>Club</t>
   </si>
@@ -970,13 +970,16 @@
     <t>Trophée Guy Giacomoni</t>
   </si>
   <si>
-    <t>Rencontre avenirs N° 2</t>
-  </si>
-  <si>
     <t>Natathlon poussins N° 1</t>
   </si>
   <si>
     <t>Golden Tour</t>
+  </si>
+  <si>
+    <t>Inter-national</t>
+  </si>
+  <si>
+    <t>Interclub Régional Minimes</t>
   </si>
   <si>
     <t>Coupe Interclubs 14 ans-15 ans</t>
@@ -1082,7 +1085,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1092,13 +1095,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFF66"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF66CCFF"/>
         <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor rgb="FFFFFF99"/>
       </patternFill>
     </fill>
   </fills>
@@ -1139,7 +1148,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1188,6 +1197,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="17" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="17" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1204,7 +1225,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFFF66"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -1273,9 +1294,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1536,18 +1557,18 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A213" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A213" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F240" activeCellId="0" sqref="F240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5051,8 +5072,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5210,19 +5231,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5461,11 +5482,13 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
-      <c r="B16" s="11" t="n">
+      <c r="A16" s="12" t="n">
+        <v>36323</v>
+      </c>
+      <c r="B16" s="13" t="n">
         <v>42386</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="14" t="s">
         <v>315</v>
       </c>
       <c r="D16" s="8" t="s">
@@ -5474,14 +5497,18 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
-      <c r="B17" s="11" t="n">
+      <c r="A17" s="12" t="n">
+        <v>36325</v>
+      </c>
+      <c r="B17" s="13" t="n">
         <v>42386</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="D17" s="8"/>
+      <c r="C17" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>301</v>
+      </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5492,29 +5519,37 @@
         <v>42393</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="D18" s="8"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
-      <c r="B19" s="11" t="n">
-        <v>42400</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D19" s="8"/>
+      <c r="A19" s="4" t="n">
+        <v>37017</v>
+      </c>
+      <c r="B19" s="9" t="n">
+        <v>42399</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>304</v>
+      </c>
       <c r="E19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
+      <c r="A20" s="4" t="n">
+        <v>37025</v>
+      </c>
       <c r="B20" s="11" t="n">
         <v>42400</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="4"/>
@@ -5522,7 +5557,7 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
       <c r="B21" s="11" t="n">
-        <v>42407</v>
+        <v>42400</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>319</v>
@@ -5533,7 +5568,7 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
       <c r="B22" s="11" t="n">
-        <v>42427</v>
+        <v>42407</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>320</v>
@@ -5542,9 +5577,11 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4"/>
+      <c r="A23" s="12" t="n">
+        <v>36327</v>
+      </c>
       <c r="B23" s="11" t="n">
-        <v>42428</v>
+        <v>42427</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>321</v>
@@ -5555,7 +5592,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="11" t="n">
-        <v>42435</v>
+        <v>42428</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>322</v>
@@ -5566,7 +5603,7 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="11" t="n">
-        <v>42442</v>
+        <v>42435</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>323</v>
@@ -5577,7 +5614,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="11" t="n">
-        <v>42449</v>
+        <v>42442</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>324</v>
@@ -5588,7 +5625,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="11" t="n">
-        <v>42456</v>
+        <v>42449</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>325</v>
@@ -5599,10 +5636,10 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="11" t="n">
-        <v>42462</v>
+        <v>42456</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="4"/>
@@ -5610,10 +5647,10 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="11" t="n">
-        <v>42463</v>
+        <v>42462</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="4"/>
@@ -5621,7 +5658,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="11" t="n">
-        <v>42470</v>
+        <v>42463</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>327</v>
@@ -5632,7 +5669,7 @@
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
       <c r="B31" s="11" t="n">
-        <v>42484</v>
+        <v>42470</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>328</v>
@@ -5643,7 +5680,7 @@
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
       <c r="B32" s="11" t="n">
-        <v>42498</v>
+        <v>42484</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>329</v>
@@ -5654,7 +5691,7 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
       <c r="B33" s="11" t="n">
-        <v>42505</v>
+        <v>42498</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>330</v>
@@ -5665,7 +5702,7 @@
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="11" t="n">
-        <v>42512</v>
+        <v>42505</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>331</v>
@@ -5687,7 +5724,7 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
       <c r="B36" s="11" t="n">
-        <v>42526</v>
+        <v>42512</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>333</v>
@@ -5698,7 +5735,7 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
       <c r="B37" s="11" t="n">
-        <v>42160</v>
+        <v>42526</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>334</v>
@@ -5709,7 +5746,7 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
       <c r="B38" s="11" t="n">
-        <v>42167</v>
+        <v>42160</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>335</v>
@@ -5720,7 +5757,7 @@
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4"/>
       <c r="B39" s="11" t="n">
-        <v>42174</v>
+        <v>42167</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>336</v>
@@ -5742,7 +5779,7 @@
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4"/>
       <c r="B41" s="11" t="n">
-        <v>42180</v>
+        <v>42174</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>338</v>
@@ -5750,9 +5787,21 @@
       <c r="D41" s="8"/>
       <c r="E41" s="4"/>
     </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+      <c r="B42" s="11" t="n">
+        <v>42180</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D41" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D42" type="list">
       <formula1>"Départemental,Régional,National 2,National,Inter-national"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Add more export for finance
</commit_message>
<xml_diff>
--- a/Officiels.xlsx
+++ b/Officiels.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Clubs" sheetId="1" state="visible" r:id="rId2"/>
@@ -1816,16 +1816,15 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1951,7 +1950,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>635</v>
+        <v>1460</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>14</v>
@@ -2083,7 +2082,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>1460</v>
+        <v>635</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>26</v>
@@ -2138,8 +2137,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2388,7 +2387,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2509,7 +2508,8 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2777,8 +2777,9 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3135,7 +3136,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3204,16 +3207,16 @@
   </sheetPr>
   <dimension ref="A1:F124"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C120" activeCellId="0" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4605,9 +4608,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5914,9 +5917,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add new information and compétition types
</commit_message>
<xml_diff>
--- a/Officiels.xlsx
+++ b/Officiels.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Clubs" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="690">
   <si>
     <t xml:space="preserve">Index</t>
   </si>
@@ -1103,13 +1103,22 @@
     <t xml:space="preserve">Gymnasiades</t>
   </si>
   <si>
-    <t xml:space="preserve">Championnats N2 Hiver Q1 (avec épreuve suppplémentaire)</t>
+    <t xml:space="preserve">Championnats N2 Hiver Q1 (avec épreuve supplémentaire)</t>
   </si>
   <si>
     <t xml:space="preserve">Championnats de Nationale 2 Hiver Q1 (Dom-Tom)</t>
   </si>
   <si>
     <t xml:space="preserve">Championnat Régional Hiver 50m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Championnats de Nationale 3 Printemps Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Championnats Régionaux en grand bassin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Championnats Régionaux Sud de Printemps Open - 50 m</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -2278,12 +2287,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2359,12 +2368,10 @@
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3225,22 +3232,20 @@
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.21875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3248,10 +3253,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3259,10 +3264,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3270,10 +3275,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3281,10 +3286,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3292,10 +3297,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3303,10 +3308,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3314,10 +3319,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3325,10 +3330,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3336,10 +3341,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3347,10 +3352,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3358,10 +3363,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3369,10 +3374,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3380,10 +3385,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3391,10 +3396,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3402,10 +3407,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3413,10 +3418,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3424,10 +3429,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3435,10 +3440,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3446,10 +3451,10 @@
         <v>20</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3457,10 +3462,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3468,10 +3473,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3479,10 +3484,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3490,10 +3495,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3501,10 +3506,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3512,10 +3517,10 @@
         <v>26</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3523,10 +3528,10 @@
         <v>27</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3534,10 +3539,10 @@
         <v>28</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3545,10 +3550,10 @@
         <v>29</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3556,10 +3561,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3567,10 +3572,10 @@
         <v>31</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3578,10 +3583,10 @@
         <v>32</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3589,10 +3594,10 @@
         <v>33</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3600,10 +3605,10 @@
         <v>34</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3611,10 +3616,10 @@
         <v>35</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3622,10 +3627,10 @@
         <v>36</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3633,10 +3638,10 @@
         <v>37</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3644,10 +3649,10 @@
         <v>38</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3655,10 +3660,10 @@
         <v>39</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3666,10 +3671,10 @@
         <v>40</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3677,10 +3682,10 @@
         <v>41</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3688,10 +3693,10 @@
         <v>42</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3699,10 +3704,10 @@
         <v>43</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3710,10 +3715,10 @@
         <v>44</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3721,10 +3726,10 @@
         <v>45</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3732,10 +3737,10 @@
         <v>46</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3743,10 +3748,10 @@
         <v>47</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3754,10 +3759,10 @@
         <v>48</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3765,10 +3770,10 @@
         <v>49</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3776,10 +3781,10 @@
         <v>50</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3787,10 +3792,10 @@
         <v>51</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3798,10 +3803,10 @@
         <v>52</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3809,10 +3814,10 @@
         <v>53</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3820,10 +3825,10 @@
         <v>54</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3831,10 +3836,10 @@
         <v>55</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3842,10 +3847,10 @@
         <v>56</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3853,10 +3858,10 @@
         <v>57</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3864,10 +3869,10 @@
         <v>58</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3875,10 +3880,10 @@
         <v>59</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3886,10 +3891,10 @@
         <v>60</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3897,10 +3902,10 @@
         <v>61</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3908,10 +3913,10 @@
         <v>62</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3919,10 +3924,10 @@
         <v>63</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3930,10 +3935,10 @@
         <v>64</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3941,10 +3946,10 @@
         <v>65</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3952,10 +3957,10 @@
         <v>66</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3963,10 +3968,10 @@
         <v>67</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
     </row>
   </sheetData>
@@ -3974,8 +3979,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3991,20 +3996,17 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -4016,16 +4018,16 @@
         <v>194264</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="D2" s="10" t="n">
         <v>433</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4033,16 +4035,16 @@
         <v>2714367</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="D3" s="10" t="n">
         <v>278</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
     </row>
   </sheetData>
@@ -4050,8 +4052,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4067,14 +4069,12 @@
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4461,10 +4461,9 @@
       <selection pane="topLeft" activeCell="S7" activeCellId="0" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4582,11 +4581,10 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4834,8 +4832,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4851,12 +4849,11 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5194,8 +5191,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5211,12 +5208,10 @@
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5326,8 +5321,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -5337,20 +5332,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C174"/>
+  <dimension ref="A1:C177"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C175" activeCellId="0" sqref="C175"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B180" activeCellId="0" sqref="B180"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.21875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="56.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7267,13 +7260,46 @@
         <v>4</v>
       </c>
     </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="n">
+        <v>251</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="C175" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="n">
+        <v>255</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="C176" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="n">
+        <v>295</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="C177" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -7285,23 +7311,21 @@
   </sheetPr>
   <dimension ref="A1:B160"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.21875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7309,7 +7333,7 @@
         <v>100</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7317,7 +7341,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7325,7 +7349,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7333,7 +7357,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7341,7 +7365,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7349,7 +7373,7 @@
         <v>250</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7357,7 +7381,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7365,7 +7389,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7373,7 +7397,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7381,7 +7405,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7389,7 +7413,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7397,7 +7421,7 @@
         <v>110</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7405,7 +7429,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7413,7 +7437,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7421,7 +7445,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7429,7 +7453,7 @@
         <v>120</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7437,7 +7461,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7445,7 +7469,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7453,7 +7477,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7461,7 +7485,7 @@
         <v>130</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7469,7 +7493,7 @@
         <v>31</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7477,7 +7501,7 @@
         <v>32</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7485,7 +7509,7 @@
         <v>33</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7493,7 +7517,7 @@
         <v>40</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7501,7 +7525,7 @@
         <v>41</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7509,7 +7533,7 @@
         <v>252</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7517,7 +7541,7 @@
         <v>42</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7525,7 +7549,7 @@
         <v>283</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7533,7 +7557,7 @@
         <v>289</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7541,7 +7565,7 @@
         <v>295</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7549,7 +7573,7 @@
         <v>301</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7557,7 +7581,7 @@
         <v>8</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7565,7 +7589,7 @@
         <v>47</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7573,7 +7597,7 @@
         <v>43</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7581,7 +7605,7 @@
         <v>44</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7589,7 +7613,7 @@
         <v>254</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7597,7 +7621,7 @@
         <v>111</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7605,7 +7629,7 @@
         <v>256</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7613,7 +7637,7 @@
         <v>121</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7621,7 +7645,7 @@
         <v>258</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7629,7 +7653,7 @@
         <v>131</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7637,7 +7661,7 @@
         <v>39</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7645,7 +7669,7 @@
         <v>48</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7653,7 +7677,7 @@
         <v>46</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7661,7 +7685,7 @@
         <v>271</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7669,7 +7693,7 @@
         <v>49</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7677,7 +7701,7 @@
         <v>265</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7685,7 +7709,7 @@
         <v>243</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7693,7 +7717,7 @@
         <v>14</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7701,7 +7725,7 @@
         <v>277</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7709,7 +7733,7 @@
         <v>9</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7717,7 +7741,7 @@
         <v>45</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7725,7 +7749,7 @@
         <v>305</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7733,7 +7757,7 @@
         <v>150</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7741,7 +7765,7 @@
         <v>51</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7749,7 +7773,7 @@
         <v>52</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7757,7 +7781,7 @@
         <v>53</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7765,7 +7789,7 @@
         <v>54</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7773,7 +7797,7 @@
         <v>249</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7781,7 +7805,7 @@
         <v>55</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7789,7 +7813,7 @@
         <v>57</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7797,7 +7821,7 @@
         <v>56</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7805,7 +7829,7 @@
         <v>66</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7813,7 +7837,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7821,7 +7845,7 @@
         <v>160</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7829,7 +7853,7 @@
         <v>61</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7837,7 +7861,7 @@
         <v>62</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7845,7 +7869,7 @@
         <v>63</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7853,7 +7877,7 @@
         <v>170</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7861,7 +7885,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7869,7 +7893,7 @@
         <v>72</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7877,7 +7901,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7885,7 +7909,7 @@
         <v>180</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7893,7 +7917,7 @@
         <v>81</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7901,7 +7925,7 @@
         <v>82</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7909,7 +7933,7 @@
         <v>83</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7917,7 +7941,7 @@
         <v>90</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7925,7 +7949,7 @@
         <v>91</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7933,7 +7957,7 @@
         <v>251</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7941,7 +7965,7 @@
         <v>92</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7949,7 +7973,7 @@
         <v>281</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7957,7 +7981,7 @@
         <v>287</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7965,7 +7989,7 @@
         <v>293</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7973,7 +7997,7 @@
         <v>299</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7981,7 +8005,7 @@
         <v>58</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7989,7 +8013,7 @@
         <v>97</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7997,7 +8021,7 @@
         <v>93</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8005,7 +8029,7 @@
         <v>94</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8013,7 +8037,7 @@
         <v>253</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8021,7 +8045,7 @@
         <v>161</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8029,7 +8053,7 @@
         <v>255</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8037,7 +8061,7 @@
         <v>171</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8045,7 +8069,7 @@
         <v>257</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8053,7 +8077,7 @@
         <v>181</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8061,7 +8085,7 @@
         <v>89</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8069,7 +8093,7 @@
         <v>98</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8077,7 +8101,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8085,7 +8109,7 @@
         <v>273</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8093,7 +8117,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8101,7 +8125,7 @@
         <v>266</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8109,7 +8133,7 @@
         <v>244</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8117,7 +8141,7 @@
         <v>64</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8125,7 +8149,7 @@
         <v>275</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8133,7 +8157,7 @@
         <v>59</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8141,7 +8165,7 @@
         <v>95</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8149,7 +8173,7 @@
         <v>304</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8157,7 +8181,7 @@
         <v>200</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8165,7 +8189,7 @@
         <v>201</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8173,7 +8197,7 @@
         <v>202</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8181,7 +8205,7 @@
         <v>203</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8189,7 +8213,7 @@
         <v>204</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8197,7 +8221,7 @@
         <v>262</v>
       </c>
       <c r="B113" s="10" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8205,7 +8229,7 @@
         <v>205</v>
       </c>
       <c r="B114" s="10" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8213,7 +8237,7 @@
         <v>207</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8221,7 +8245,7 @@
         <v>206</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8229,7 +8253,7 @@
         <v>216</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8237,7 +8261,7 @@
         <v>215</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8245,7 +8269,7 @@
         <v>210</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8253,7 +8277,7 @@
         <v>211</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8261,7 +8285,7 @@
         <v>212</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8269,7 +8293,7 @@
         <v>213</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8277,7 +8301,7 @@
         <v>220</v>
       </c>
       <c r="B123" s="10" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8285,7 +8309,7 @@
         <v>221</v>
       </c>
       <c r="B124" s="10" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8293,7 +8317,7 @@
         <v>222</v>
       </c>
       <c r="B125" s="10" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8301,7 +8325,7 @@
         <v>223</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8309,7 +8333,7 @@
         <v>230</v>
       </c>
       <c r="B127" s="10" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8317,7 +8341,7 @@
         <v>231</v>
       </c>
       <c r="B128" s="10" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8325,7 +8349,7 @@
         <v>232</v>
       </c>
       <c r="B129" s="10" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8333,7 +8357,7 @@
         <v>233</v>
       </c>
       <c r="B130" s="10" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8341,7 +8365,7 @@
         <v>240</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8349,7 +8373,7 @@
         <v>241</v>
       </c>
       <c r="B132" s="10" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8357,7 +8381,7 @@
         <v>263</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8365,7 +8389,7 @@
         <v>242</v>
       </c>
       <c r="B134" s="10" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8373,7 +8397,7 @@
         <v>285</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8381,7 +8405,7 @@
         <v>291</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8389,7 +8413,7 @@
         <v>297</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8397,7 +8421,7 @@
         <v>303</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8405,7 +8429,7 @@
         <v>86</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8413,7 +8437,7 @@
         <v>87</v>
       </c>
       <c r="B140" s="10" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8421,7 +8445,7 @@
         <v>88</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8429,7 +8453,7 @@
         <v>34</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8437,7 +8461,7 @@
         <v>259</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8445,7 +8469,7 @@
         <v>246</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8453,7 +8477,7 @@
         <v>260</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8461,7 +8485,7 @@
         <v>247</v>
       </c>
       <c r="B146" s="10" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8469,7 +8493,7 @@
         <v>261</v>
       </c>
       <c r="B147" s="10" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8477,7 +8501,7 @@
         <v>248</v>
       </c>
       <c r="B148" s="10" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8485,7 +8509,7 @@
         <v>38</v>
       </c>
       <c r="B149" s="10" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8493,7 +8517,7 @@
         <v>37</v>
       </c>
       <c r="B150" s="10" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8501,7 +8525,7 @@
         <v>36</v>
       </c>
       <c r="B151" s="10" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8509,7 +8533,7 @@
         <v>269</v>
       </c>
       <c r="B152" s="10" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8517,7 +8541,7 @@
         <v>35</v>
       </c>
       <c r="B153" s="10" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8525,7 +8549,7 @@
         <v>267</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8533,7 +8557,7 @@
         <v>245</v>
       </c>
       <c r="B155" s="10" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8541,7 +8565,7 @@
         <v>214</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8549,7 +8573,7 @@
         <v>279</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8557,7 +8581,7 @@
         <v>84</v>
       </c>
       <c r="B158" s="10" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8565,7 +8589,7 @@
         <v>85</v>
       </c>
       <c r="B159" s="10" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8573,7 +8597,7 @@
         <v>264</v>
       </c>
       <c r="B160" s="10" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -8581,8 +8605,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -8595,44 +8619,41 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
-        <v>361</v>
-      </c>
+      <c r="A1" s="10"/>
       <c r="B1" s="11" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="B2" s="13" t="n">
         <v>0.00038275462962963</v>
@@ -8658,7 +8679,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="B3" s="13" t="n">
         <v>0.000836574074074074</v>
@@ -8684,7 +8705,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B4" s="13" t="n">
         <v>0.00182627314814815</v>
@@ -8710,7 +8731,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="B5" s="13" t="n">
         <v>0.00387974537037037</v>
@@ -8736,7 +8757,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="B6" s="13" t="n">
         <v>0.00797337962962963</v>
@@ -8762,7 +8783,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B7" s="13" t="n">
         <v>0.0149025462962963</v>
@@ -8788,7 +8809,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="B8" s="13" t="n">
         <v>0.000447453703703704</v>
@@ -8814,7 +8835,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="B9" s="13" t="n">
         <v>0.000994212962962963</v>
@@ -8840,7 +8861,7 @@
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="B10" s="13" t="n">
         <v>0.00205451388888889</v>
@@ -8866,7 +8887,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="B11" s="13" t="n">
         <v>0.000488194444444444</v>
@@ -8892,7 +8913,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="B12" s="13" t="n">
         <v>0.00110046296296296</v>
@@ -8918,7 +8939,7 @@
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B13" s="13" t="n">
         <v>0.00233414351851852</v>
@@ -8944,7 +8965,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="B14" s="13" t="n">
         <v>0.000405671296296296</v>
@@ -8970,7 +8991,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="B15" s="13" t="n">
         <v>0.000929861111111111</v>
@@ -8996,7 +9017,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="B16" s="13" t="n">
         <v>0.0020375</v>
@@ -9022,7 +9043,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="B17" s="13" t="n">
         <v>0.0021537037037037</v>
@@ -9048,7 +9069,7 @@
     </row>
     <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="B18" s="13" t="n">
         <v>0.00442303240740741</v>
@@ -9077,8 +9098,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normál"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normál"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>